<commit_message>
updated requirements, docker related files and ran dag for 15t news insights
</commit_message>
<xml_diff>
--- a/other/tasks.xlsx
+++ b/other/tasks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\News-Project\Stock-Sentiment-Analysis-With-Airflow-and-Google-Gemini\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\News-Project\Stock-Sentiment-Analysis-with-Apache-Airflow-and-Google-Gemini\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098BF8CF-C6FC-4545-B623-43069F3872A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A058717-5A68-4779-8B65-94165C455F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Task</t>
   </si>
@@ -95,6 +95,13 @@
   </si>
   <si>
     <t>It just gets added as new tasks and for those ran earlier, it's blank there but when you clear the task just before the added ones, the new ones all run.</t>
+  </si>
+  <si>
+    <t>Issues/Comments</t>
+  </si>
+  <si>
+    <t>Connecting to vertica from the docker container isn't working, need to think about how to make It work for both DBT and the normal data loading.
+I think what I need to do is make the vertica DB accessible over the web and update the readme</t>
   </si>
 </sst>
 </file>
@@ -478,14 +485,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="84.85546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="63.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -498,6 +508,9 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -656,7 +669,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -665,6 +678,9 @@
       </c>
       <c r="C16" t="s">
         <v>14</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added libgompl to installed libraries by root user
</commit_message>
<xml_diff>
--- a/other/tasks.xlsx
+++ b/other/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\News-Project\Stock-Sentiment-Analysis-with-Apache-Airflow-and-Google-Gemini\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A058717-5A68-4779-8B65-94165C455F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74A3D75-F8C2-4B2F-9B65-06AAD4EAD3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,8 @@
   </si>
   <si>
     <t>Connecting to vertica from the docker container isn't working, need to think about how to make It work for both DBT and the normal data loading.
-I think what I need to do is make the vertica DB accessible over the web and update the readme</t>
+I think what I need to do is make the vertica DB accessible over the web and update the readme
+Light gbm gave an issue so I had to install some other lightgb library as root and added to the docker file</t>
   </si>
 </sst>
 </file>
@@ -488,7 +489,7 @@
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,7 +670,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>